<commit_message>
Aggiunta tabella Habitat, aggiunta tabella Zona con morfologie per le query, aggiunte tutte funzioni tranne la 3 nel file sql
</commit_message>
<xml_diff>
--- a/FileInputScript/Zone/TabellafIN.xlsx
+++ b/FileInputScript/Zone/TabellafIN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="145">
   <si>
     <t xml:space="preserve">Accademia Team Rocket</t>
   </si>
@@ -31,15 +31,24 @@
     <t xml:space="preserve">\N</t>
   </si>
   <si>
+    <t xml:space="preserve">Edificio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accettazione Lega Pokémon</t>
   </si>
   <si>
     <t xml:space="preserve">Albero dell'Inizio</t>
   </si>
   <si>
+    <t xml:space="preserve">Grotta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Altopiano Blu</t>
   </si>
   <si>
+    <t xml:space="preserve">Prateria</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aranciopoli</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Casa delle Memorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acqua</t>
   </si>
   <si>
     <t xml:space="preserve">Casa di Duplica</t>
@@ -803,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E147" activeCellId="0" sqref="E147"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C149" activeCellId="0" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -828,7 +840,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,7 +848,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>1</v>
@@ -845,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>1</v>
@@ -862,7 +874,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>1</v>
@@ -879,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +899,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>1</v>
@@ -896,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>1</v>
@@ -913,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,7 +933,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>1</v>
@@ -930,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +950,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>1</v>
@@ -947,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>1</v>
@@ -964,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,7 +984,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>1</v>
@@ -981,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,7 +1001,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>1</v>
@@ -998,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,7 +1018,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>1</v>
@@ -1015,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,7 +1035,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>1</v>
@@ -1032,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,7 +1052,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>1</v>
@@ -1049,7 +1061,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,7 +1069,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>1</v>
@@ -1066,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,7 +1086,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>1</v>
@@ -1083,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,7 +1103,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>1</v>
@@ -1100,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,7 +1120,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>1</v>
@@ -1117,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,7 +1137,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>1</v>
@@ -1134,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,7 +1154,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>1</v>
@@ -1151,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,7 +1171,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>1</v>
@@ -1168,7 +1180,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,7 +1188,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>1</v>
@@ -1185,7 +1197,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1205,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>1</v>
@@ -1202,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,7 +1222,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>1</v>
@@ -1219,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,7 +1239,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>1</v>
@@ -1236,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,7 +1256,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>1</v>
@@ -1253,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,7 +1273,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>1</v>
@@ -1270,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,7 +1290,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>1</v>
@@ -1287,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,7 +1307,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>1</v>
@@ -1304,7 +1316,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,7 +1324,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>1</v>
@@ -1321,7 +1333,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,7 +1341,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>1</v>
@@ -1338,7 +1350,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,7 +1358,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>1</v>
@@ -1355,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,7 +1375,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>1</v>
@@ -1372,7 +1384,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1392,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>1</v>
@@ -1389,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,7 +1409,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>1</v>
@@ -1406,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,7 +1426,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>1</v>
@@ -1423,7 +1435,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,7 +1443,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>1</v>
@@ -1440,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,7 +1460,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>1</v>
@@ -1457,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,7 +1477,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>1</v>
@@ -1474,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,7 +1494,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>1</v>
@@ -1491,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1499,7 +1511,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>1</v>
@@ -1508,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1528,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>1</v>
@@ -1525,7 +1537,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,7 +1545,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>1</v>
@@ -1542,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,7 +1562,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>1</v>
@@ -1559,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1579,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>1</v>
@@ -1576,7 +1588,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,7 +1596,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>1</v>
@@ -1593,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1613,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>1</v>
@@ -1610,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,7 +1630,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>1</v>
@@ -1627,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,7 +1647,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>1</v>
@@ -1644,7 +1656,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1664,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>1</v>
@@ -1661,7 +1673,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1698,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>1</v>
@@ -1695,7 +1707,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,7 +1715,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>1</v>
@@ -1712,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1732,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>1</v>
@@ -1729,7 +1741,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,7 +1749,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>1</v>
@@ -1746,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,7 +1766,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>1</v>
@@ -1763,7 +1775,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1783,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>1</v>
@@ -1780,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +1800,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>1</v>
@@ -1797,7 +1809,7 @@
         <v>2</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,7 +1817,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>1</v>
@@ -1814,7 +1826,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1834,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>1</v>
@@ -1831,7 +1843,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1851,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>1</v>
@@ -1848,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,7 +1868,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>1</v>
@@ -1865,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,7 +1885,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>1</v>
@@ -1882,7 +1894,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1902,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>1</v>
@@ -1899,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,7 +1919,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>1</v>
@@ -1916,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,7 +1936,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>1</v>
@@ -1933,7 +1945,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1941,7 +1953,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>1</v>
@@ -1950,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,7 +1970,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>1</v>
@@ -1967,7 +1979,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1975,7 +1987,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>1</v>
@@ -1984,7 +1996,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,7 +2004,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>1</v>
@@ -2001,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,7 +2021,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>1</v>
@@ -2018,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2038,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>1</v>
@@ -2035,7 +2047,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,7 +2055,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>1</v>
@@ -2052,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2060,7 +2072,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>1</v>
@@ -2069,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,7 +2089,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>1</v>
@@ -2086,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2094,7 +2106,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>1</v>
@@ -2103,7 +2115,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,7 +2123,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>1</v>
@@ -2120,7 +2132,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2128,7 +2140,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>1</v>
@@ -2137,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2157,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>1</v>
@@ -2154,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2162,7 +2174,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>1</v>
@@ -2171,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,7 +2191,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>1</v>
@@ -2188,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2208,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>1</v>
@@ -2205,7 +2217,7 @@
         <v>2</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,7 +2225,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>1</v>
@@ -2222,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,7 +2242,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>1</v>
@@ -2239,7 +2251,7 @@
         <v>2</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,7 +2259,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>1</v>
@@ -2256,7 +2268,7 @@
         <v>2</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,7 +2276,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>1</v>
@@ -2273,7 +2285,7 @@
         <v>2</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,7 +2293,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>1</v>
@@ -2290,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,7 +2310,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>1</v>
@@ -2307,7 +2319,7 @@
         <v>2</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,7 +2327,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>1</v>
@@ -2324,7 +2336,7 @@
         <v>2</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2332,7 +2344,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>1</v>
@@ -2341,7 +2353,7 @@
         <v>2</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2349,7 +2361,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>1</v>
@@ -2358,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,7 +2378,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>1</v>
@@ -2375,7 +2387,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,7 +2395,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>1</v>
@@ -2392,7 +2404,7 @@
         <v>2</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2412,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>1</v>
@@ -2409,7 +2421,7 @@
         <v>2</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2417,7 +2429,7 @@
         <v>95</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>1</v>
@@ -2426,7 +2438,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,7 +2446,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>1</v>
@@ -2443,7 +2455,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2463,7 @@
         <v>97</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>1</v>
@@ -2460,7 +2472,7 @@
         <v>2</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,7 +2480,7 @@
         <v>98</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>1</v>
@@ -2477,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,7 +2497,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>1</v>
@@ -2494,7 +2506,7 @@
         <v>2</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,7 +2514,7 @@
         <v>100</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>1</v>
@@ -2511,7 +2523,7 @@
         <v>2</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2519,7 +2531,7 @@
         <v>101</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>1</v>
@@ -2528,7 +2540,7 @@
         <v>2</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2536,7 +2548,7 @@
         <v>102</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>1</v>
@@ -2545,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,7 +2565,7 @@
         <v>103</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>1</v>
@@ -2562,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2582,7 @@
         <v>104</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>1</v>
@@ -2579,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,7 +2599,7 @@
         <v>105</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>1</v>
@@ -2596,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,7 +2616,7 @@
         <v>106</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>1</v>
@@ -2613,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,7 +2633,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>1</v>
@@ -2630,7 +2642,7 @@
         <v>2</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2650,7 @@
         <v>108</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>1</v>
@@ -2647,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2655,7 +2667,7 @@
         <v>109</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>1</v>
@@ -2664,7 +2676,7 @@
         <v>2</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,7 +2684,7 @@
         <v>110</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>1</v>
@@ -2681,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,7 +2701,7 @@
         <v>111</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>1</v>
@@ -2698,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,7 +2718,7 @@
         <v>112</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>1</v>
@@ -2715,7 +2727,7 @@
         <v>2</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,7 +2735,7 @@
         <v>113</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>1</v>
@@ -2732,7 +2744,7 @@
         <v>2</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,7 +2752,7 @@
         <v>114</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>1</v>
@@ -2749,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,7 +2769,7 @@
         <v>115</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>1</v>
@@ -2766,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,7 +2786,7 @@
         <v>116</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>1</v>
@@ -2783,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,7 +2803,7 @@
         <v>117</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>1</v>
@@ -2800,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,7 +2820,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>1</v>
@@ -2817,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2825,7 +2837,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>1</v>
@@ -2834,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2842,7 +2854,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>1</v>
@@ -2851,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,7 +2871,7 @@
         <v>121</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>1</v>
@@ -2868,7 +2880,7 @@
         <v>2</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2876,7 +2888,7 @@
         <v>122</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C122" s="0" t="s">
         <v>1</v>
@@ -2885,7 +2897,7 @@
         <v>2</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,7 +2905,7 @@
         <v>123</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>1</v>
@@ -2902,7 +2914,7 @@
         <v>2</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2910,7 +2922,7 @@
         <v>124</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>1</v>
@@ -2919,7 +2931,7 @@
         <v>2</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,7 +2939,7 @@
         <v>125</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>1</v>
@@ -2936,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2944,7 +2956,7 @@
         <v>126</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>1</v>
@@ -2953,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,7 +2973,7 @@
         <v>127</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>1</v>
@@ -2970,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,7 +2990,7 @@
         <v>128</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>1</v>
@@ -2987,7 +2999,7 @@
         <v>2</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,7 +3007,7 @@
         <v>129</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C129" s="0" t="s">
         <v>1</v>
@@ -3004,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3012,7 +3024,7 @@
         <v>130</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C130" s="0" t="s">
         <v>1</v>
@@ -3021,7 +3033,7 @@
         <v>2</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,7 +3041,7 @@
         <v>131</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C131" s="0" t="s">
         <v>1</v>
@@ -3038,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,7 +3058,7 @@
         <v>132</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>1</v>
@@ -3055,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3063,7 +3075,7 @@
         <v>133</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>1</v>
@@ -3072,7 +3084,7 @@
         <v>2</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3080,7 +3092,7 @@
         <v>134</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>1</v>
@@ -3089,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,7 +3109,7 @@
         <v>135</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>1</v>
@@ -3106,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,7 +3126,7 @@
         <v>136</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C136" s="0" t="s">
         <v>1</v>
@@ -3123,7 +3135,7 @@
         <v>2</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,7 +3143,7 @@
         <v>137</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>1</v>
@@ -3140,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3160,7 @@
         <v>138</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>1</v>
@@ -3157,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="E138" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,7 +3177,7 @@
         <v>139</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C139" s="0" t="s">
         <v>1</v>
@@ -3174,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3182,7 +3194,7 @@
         <v>140</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>1</v>
@@ -3191,7 +3203,7 @@
         <v>2</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>